<commit_message>
adição do testng.xml, driver factory, finazlicação dos cenários e refatoração
</commit_message>
<xml_diff>
--- a/excel/ExcelData.xlsx
+++ b/excel/ExcelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emerson.prado\eclipse-toolsqa\workspace-cucumber\ProjetoLoja\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C030ED7-7A40-4465-85D4-FEAC4EF75406}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EE2DB4-6C97-44F9-81F3-C51003566435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{62909120-00D7-4069-A6D0-EEC82528B5AC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Produto</t>
   </si>
@@ -44,12 +44,6 @@
     <t>TestCase_ID</t>
   </si>
   <si>
-    <t>Tablet</t>
-  </si>
-  <si>
-    <t>Sucesso</t>
-  </si>
-  <si>
     <t>Laptop</t>
   </si>
   <si>
@@ -60,6 +54,9 @@
   </si>
   <si>
     <t>Teste4</t>
+  </si>
+  <si>
+    <t>HP ElitePad 1000 G2 Tablet</t>
   </si>
 </sst>
 </file>
@@ -433,7 +430,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,10 +453,10 @@
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -467,10 +464,10 @@
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -478,17 +475,19 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Finalização do projeto TDD
</commit_message>
<xml_diff>
--- a/excel/ExcelData.xlsx
+++ b/excel/ExcelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emerson.prado\eclipse-toolsqa\workspace-cucumber\ProjetoLoja\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04EE2DB4-6C97-44F9-81F3-C51003566435}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950D878C-4DBA-4FF3-8434-553EAD6E324F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{62909120-00D7-4069-A6D0-EEC82528B5AC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
   <si>
     <t>Produto</t>
   </si>
@@ -50,13 +50,13 @@
     <t>Funcionou</t>
   </si>
   <si>
-    <t>Teste3</t>
-  </si>
-  <si>
     <t>Teste4</t>
   </si>
   <si>
     <t>HP ElitePad 1000 G2 Tablet</t>
+  </si>
+  <si>
+    <t>Invalid Search</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +453,7 @@
     </row>
     <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>

</xml_diff>